<commit_message>
finished hte base case model: there are some placeholders used, particularly in utilites and mortality cost, but this is fixed shortly
</commit_message>
<xml_diff>
--- a/results/calculate.icers.xlsx
+++ b/results/calculate.icers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayman\Google Drive\research\trauma\CT.neck\code\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{059A396C-5558-4592-8C9A-CDB2445B3DEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3CA401-58EC-4F4D-B5D8-C67FF8D90074}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{555142B4-3F8F-4AF8-A607-9B3B2C08214D}"/>
+    <workbookView xWindow="1185" yWindow="-120" windowWidth="27735" windowHeight="16440" xr2:uid="{555142B4-3F8F-4AF8-A607-9B3B2C08214D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>ICER calcaulation</t>
   </si>
@@ -470,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEC1D9CD-8320-4D51-AC57-CBFEF8360549}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B18" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,6 +830,88 @@
         <v>19</v>
       </c>
     </row>
+    <row r="32" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>3</v>
+      </c>
+      <c r="H32" t="s">
+        <v>1</v>
+      </c>
+      <c r="I32" t="s">
+        <v>2</v>
+      </c>
+      <c r="J32" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>7</v>
+      </c>
+      <c r="H33">
+        <v>24177.5805553879</v>
+      </c>
+      <c r="I33">
+        <v>0.61573595541761295</v>
+      </c>
+      <c r="J33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>5</v>
+      </c>
+      <c r="H34">
+        <v>24178.360498779901</v>
+      </c>
+      <c r="I34">
+        <v>0.61751482912255096</v>
+      </c>
+      <c r="J34">
+        <v>438.44787285111875</v>
+      </c>
+    </row>
+    <row r="35" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>6</v>
+      </c>
+      <c r="H35">
+        <v>24241.862419323399</v>
+      </c>
+      <c r="I35">
+        <v>0.62051449850734697</v>
+      </c>
+      <c r="J35">
+        <v>21169.639849431824</v>
+      </c>
+    </row>
+    <row r="36" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G36" t="s">
+        <v>4</v>
+      </c>
+      <c r="H36">
+        <v>24568.2377349134</v>
+      </c>
+      <c r="I36">
+        <v>0.62492680289312497</v>
+      </c>
+      <c r="J36">
+        <v>73969.356384839077</v>
+      </c>
+    </row>
+    <row r="38" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H38">
+        <f>I36-I33</f>
+        <v>9.1908474755120206E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="H39">
+        <f>H38*1000</f>
+        <v>9.1908474755120206</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>